<commit_message>
Supports EPV. Include responder for text-related questions in the spreadsheets generated
</commit_message>
<xml_diff>
--- a/question_definitions.xlsx
+++ b/question_definitions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chang Kiat\Desktop\Others\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\data-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E717D3-1EBF-4024-AE91-278D89CA0495}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606A406E-A45C-4D90-9D22-3D5B7137CB20}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3771" yWindow="3771" windowWidth="24686" windowHeight="13080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Free Text</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>Type</t>
+  </si>
+  <si>
+    <t>epv</t>
+  </si>
+  <si>
+    <t>Table (A,B,C,D)</t>
   </si>
 </sst>
 </file>
@@ -372,9 +378,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
@@ -421,6 +429,14 @@
         <v>7</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added another type of question to process
</commit_message>
<xml_diff>
--- a/question_definitions.xlsx
+++ b/question_definitions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\data-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606A406E-A45C-4D90-9D22-3D5B7137CB20}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36DE0253-C519-4469-9ED0-FBAAE66E9A30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Free Text</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>Table (A,B,C,D)</t>
+  </si>
+  <si>
+    <t>Table2</t>
+  </si>
+  <si>
+    <t>websitefeature</t>
   </si>
 </sst>
 </file>
@@ -378,11 +384,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
@@ -437,6 +441,14 @@
         <v>10</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Print the full name of the question type below every question
</commit_message>
<xml_diff>
--- a/question_definitions.xlsx
+++ b/question_definitions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\data-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36DE0253-C519-4469-9ED0-FBAAE66E9A30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B14E6DA1-EC4C-41DC-865F-7055D6C326D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4663" yWindow="3943" windowWidth="24686" windowHeight="13080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
     <t>Table2</t>
   </si>
   <si>
-    <t>websitefeature</t>
+    <t>wf</t>
   </si>
 </sst>
 </file>

</xml_diff>